<commit_message>
Atualização planilha de homologação
</commit_message>
<xml_diff>
--- a/Documentação/Plano de UAT - Homol 1 Semestre 2019 v1.xlsx
+++ b/Documentação/Plano de UAT - Homol 1 Semestre 2019 v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C98F7A-E248-40B8-A72D-EAF910D19D6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FB7C83-47C5-477D-9C73-4B2322F1D8C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="503" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="195">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -501,9 +501,6 @@
     <t>RF001-01</t>
   </si>
   <si>
-    <t>Permitir o cadastro no sistema utilizando Nome completo, email, senha, confirmar senha, CPF/CNPJ, CEP, rua, número, número da casa, complemento, tamanho(m2), quantidade de ar-condicionado e potência média.</t>
-  </si>
-  <si>
     <t>Permitir autenticação de usuários com os campos indicados corretamente para cadastra-los no banco de dados.</t>
   </si>
   <si>
@@ -561,9 +558,6 @@
     <t>RF001-14</t>
   </si>
   <si>
-    <t>RF001-15</t>
-  </si>
-  <si>
     <t>Consistir campo "email" para coletar o email do cliente.</t>
   </si>
   <si>
@@ -571,6 +565,75 @@
   </si>
   <si>
     <t>Permitir que o usuário continue cadastrando seus dados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consistir campo "razão social" para coletar o nome da empresa do cliente. </t>
+  </si>
+  <si>
+    <t>Permitir a digitação do nome da empresa do cliente para cadastrar no sistema.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação de uma senha de usuário com no mínimo 8 caracteres.</t>
+  </si>
+  <si>
+    <t>Consistir campo "senha" para coletar a senha do usuário.</t>
+  </si>
+  <si>
+    <t>Consistir campo "confirmar senha" para coletar a senha de comparação do usuário.</t>
+  </si>
+  <si>
+    <t>Permirir a digitação de uma senha de usuário com no mínimo 8 carácteres para comparação com a senha do campo anterior.</t>
+  </si>
+  <si>
+    <t>Consistir campo "cpf/cnpj" para coletar o registro do usuário ou da empresa cliente que estaremos cadastrando no sistema.</t>
+  </si>
+  <si>
+    <t>Permirir a digitação do cadastro de pessoa fisíca ou cadastro nacional de pessoa juridica, desde que um deles seja válido.</t>
+  </si>
+  <si>
+    <t>Consistir campo "CEP" para coletar o endereço do usuário.</t>
+  </si>
+  <si>
+    <t>Permitir digitação de CEP(válido) para cadastro do endereço do cliente na base de dados.</t>
+  </si>
+  <si>
+    <t>Consistir campo "rua" para mostrar a rua correspondente ao CEP digitado no campo anterior</t>
+  </si>
+  <si>
+    <t>Permitir a visualização da rua correspondente ao CEP digitado no campo anterior.</t>
+  </si>
+  <si>
+    <t>Consistir campo "numero" para coletar o numero especifico do endereço do cliente.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação do número do endereço do cliente.</t>
+  </si>
+  <si>
+    <t>Consistir campo "complemento" para coletar alguma informação adicional do endereço do cliente.</t>
+  </si>
+  <si>
+    <t>Consistir campo "apelido do galpão" para coletar um nome de identificação do galpão.</t>
+  </si>
+  <si>
+    <t>Consistir campo "tamanho(2)" para coletar o tamanho em metros quadrados do galpão.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação de um apelido do galpão para cadastro e identicação do galpão para o cliente.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação do complemento do endereço co cliente.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação do tamanho do galpão em metros quadrados e cadastra-los no banco de dados.</t>
+  </si>
+  <si>
+    <t>Consistir campo "quantidade de ar condicionados" para coletar estas informações do galpão do cliente.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação da quantidade de ar condicionados que existem no galpão.</t>
+  </si>
+  <si>
+    <t>Permitir o cadastro no sistema utilizando Nome completo, razão social, email, senha, confirmar senha, CPF/CNPJ, CEP, rua, número, complemento, apelido do galpão, tamanho(m2), quantidade de ar-condicionado.</t>
   </si>
 </sst>
 </file>
@@ -865,7 +928,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1290,6 +1353,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0">
@@ -1338,7 +1453,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1573,6 +1688,170 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="33" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1582,74 +1861,71 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1682,196 +1958,107 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2424,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2462,13 +2649,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="111"/>
       <c r="G2" s="57"/>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
@@ -2478,11 +2665,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="53"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="95"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="114"/>
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -2509,10 +2696,10 @@
       <c r="B5" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="115" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="89"/>
+      <c r="D5" s="116"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
       <c r="G5" s="28"/>
@@ -2527,10 +2714,10 @@
       <c r="B6" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="88">
+      <c r="C6" s="115">
         <v>151849</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="116"/>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
       <c r="G6" s="28"/>
@@ -2545,8 +2732,8 @@
       <c r="B7" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="116"/>
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
       <c r="G7" s="28"/>
@@ -2561,10 +2748,10 @@
       <c r="B8" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="115" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="89"/>
+      <c r="D8" s="116"/>
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
       <c r="G8" s="28"/>
@@ -2579,10 +2766,10 @@
       <c r="B9" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="106">
+      <c r="C9" s="117">
         <v>43598</v>
       </c>
-      <c r="D9" s="107"/>
+      <c r="D9" s="118"/>
       <c r="E9" s="28"/>
       <c r="F9" s="29"/>
       <c r="G9" s="28"/>
@@ -2608,16 +2795,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="74"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="121"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="24"/>
@@ -2629,14 +2816,14 @@
       <c r="B12" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="83" t="s">
+      <c r="D12" s="89"/>
+      <c r="E12" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="84"/>
+      <c r="F12" s="89"/>
       <c r="G12" s="69" t="s">
         <v>25</v>
       </c>
@@ -2659,18 +2846,18 @@
       <c r="B13" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="80" t="s">
+      <c r="D13" s="95"/>
+      <c r="E13" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="85"/>
+      <c r="F13" s="101"/>
       <c r="G13" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="H13" s="108">
+      <c r="H13" s="72">
         <v>43599</v>
       </c>
       <c r="I13" s="64" t="s">
@@ -2689,18 +2876,18 @@
       <c r="B14" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="86" t="s">
+      <c r="D14" s="93"/>
+      <c r="E14" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="87"/>
+      <c r="F14" s="103"/>
       <c r="G14" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="109">
+      <c r="H14" s="73">
         <v>43598</v>
       </c>
       <c r="I14" s="71" t="s">
@@ -2719,18 +2906,18 @@
       <c r="B15" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="77" t="s">
+      <c r="D15" s="95"/>
+      <c r="E15" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="79"/>
+      <c r="F15" s="104"/>
       <c r="G15" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="H15" s="108">
+      <c r="H15" s="72">
         <v>43600</v>
       </c>
       <c r="I15" s="64" t="s">
@@ -2749,10 +2936,10 @@
       <c r="B16" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="77"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="79"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="104"/>
       <c r="G16" s="64"/>
       <c r="H16" s="64"/>
       <c r="I16" s="64"/>
@@ -2784,41 +2971,41 @@
     </row>
     <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="55"/>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="54"/>
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="114" t="s">
+      <c r="C19" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="115"/>
-      <c r="E19" s="114" t="s">
+      <c r="D19" s="97"/>
+      <c r="E19" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="115"/>
-      <c r="G19" s="114" t="s">
+      <c r="F19" s="97"/>
+      <c r="G19" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="115"/>
-      <c r="I19" s="113" t="s">
+      <c r="H19" s="97"/>
+      <c r="I19" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="113" t="s">
+      <c r="J19" s="75" t="s">
         <v>30</v>
       </c>
       <c r="K19" s="27"/>
@@ -2830,25 +3017,25 @@
     </row>
     <row r="20" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="136" t="s">
+      <c r="C20" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="137"/>
-      <c r="E20" s="138" t="s">
+      <c r="D20" s="108"/>
+      <c r="E20" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="139"/>
-      <c r="G20" s="138" t="s">
+      <c r="F20" s="99"/>
+      <c r="G20" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="139"/>
-      <c r="I20" s="140" t="s">
+      <c r="H20" s="99"/>
+      <c r="I20" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="J20" s="141" t="s">
+      <c r="J20" s="80" t="s">
         <v>129</v>
       </c>
       <c r="K20" s="27"/>
@@ -2860,25 +3047,25 @@
     </row>
     <row r="21" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
-      <c r="B21" s="142" t="s">
+      <c r="B21" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="116" t="s">
+      <c r="C21" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="116"/>
-      <c r="E21" s="118" t="s">
+      <c r="D21" s="90"/>
+      <c r="E21" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="118"/>
-      <c r="G21" s="119" t="s">
+      <c r="F21" s="91"/>
+      <c r="G21" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="H21" s="119"/>
-      <c r="I21" s="110" t="s">
+      <c r="H21" s="87"/>
+      <c r="I21" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="J21" s="143" t="s">
+      <c r="J21" s="82" t="s">
         <v>129</v>
       </c>
       <c r="K21" s="27"/>
@@ -2890,25 +3077,25 @@
     </row>
     <row r="22" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="116" t="s">
+      <c r="C22" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="116"/>
-      <c r="E22" s="118" t="s">
+      <c r="D22" s="90"/>
+      <c r="E22" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="118"/>
-      <c r="G22" s="119" t="s">
+      <c r="F22" s="91"/>
+      <c r="G22" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="119"/>
-      <c r="I22" s="110" t="s">
+      <c r="H22" s="87"/>
+      <c r="I22" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="J22" s="143" t="s">
+      <c r="J22" s="82" t="s">
         <v>129</v>
       </c>
       <c r="K22" s="27"/>
@@ -2920,25 +3107,25 @@
     </row>
     <row r="23" spans="1:21" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="54"/>
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="117"/>
-      <c r="E23" s="118" t="s">
+      <c r="D23" s="122"/>
+      <c r="E23" s="91" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="120"/>
-      <c r="G23" s="119" t="s">
+      <c r="F23" s="123"/>
+      <c r="G23" s="87" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="119"/>
-      <c r="I23" s="110" t="s">
+      <c r="H23" s="87"/>
+      <c r="I23" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="J23" s="143" t="s">
+      <c r="J23" s="82" t="s">
         <v>129</v>
       </c>
       <c r="K23" s="27"/>
@@ -2950,25 +3137,25 @@
     </row>
     <row r="24" spans="1:21" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="54"/>
-      <c r="B24" s="142" t="s">
+      <c r="B24" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="116" t="s">
+      <c r="C24" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="116"/>
-      <c r="E24" s="118" t="s">
+      <c r="D24" s="90"/>
+      <c r="E24" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="118"/>
-      <c r="G24" s="119" t="s">
+      <c r="F24" s="91"/>
+      <c r="G24" s="87" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="119"/>
-      <c r="I24" s="110" t="s">
+      <c r="H24" s="87"/>
+      <c r="I24" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="J24" s="143" t="s">
+      <c r="J24" s="82" t="s">
         <v>136</v>
       </c>
       <c r="K24" s="27"/>
@@ -2980,25 +3167,25 @@
     </row>
     <row r="25" spans="1:21" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
-      <c r="B25" s="142" t="s">
+      <c r="B25" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="116" t="s">
+      <c r="C25" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="116"/>
-      <c r="E25" s="118" t="s">
+      <c r="D25" s="90"/>
+      <c r="E25" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="118"/>
-      <c r="G25" s="119" t="s">
+      <c r="F25" s="91"/>
+      <c r="G25" s="87" t="s">
         <v>138</v>
       </c>
-      <c r="H25" s="119"/>
-      <c r="I25" s="110" t="s">
+      <c r="H25" s="87"/>
+      <c r="I25" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="J25" s="143" t="s">
+      <c r="J25" s="82" t="s">
         <v>129</v>
       </c>
       <c r="K25" s="27"/>
@@ -3010,25 +3197,25 @@
     </row>
     <row r="26" spans="1:21" s="4" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="54"/>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="83" t="s">
         <v>148</v>
       </c>
-      <c r="C26" s="145" t="s">
+      <c r="C26" s="124" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="146" t="s">
+      <c r="D26" s="124"/>
+      <c r="E26" s="125" t="s">
         <v>142</v>
       </c>
-      <c r="F26" s="146"/>
-      <c r="G26" s="147" t="s">
+      <c r="F26" s="125"/>
+      <c r="G26" s="126" t="s">
         <v>143</v>
       </c>
-      <c r="H26" s="147"/>
-      <c r="I26" s="148" t="s">
+      <c r="H26" s="126"/>
+      <c r="I26" s="84" t="s">
         <v>128</v>
       </c>
-      <c r="J26" s="149" t="s">
+      <c r="J26" s="85" t="s">
         <v>129</v>
       </c>
       <c r="K26" s="27"/>
@@ -3040,25 +3227,25 @@
     </row>
     <row r="27" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
-      <c r="B27" s="127" t="s">
+      <c r="B27" s="156" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="128" t="s">
+      <c r="C27" s="157" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="158"/>
+      <c r="E27" s="159" t="s">
         <v>150</v>
       </c>
-      <c r="D27" s="129"/>
-      <c r="E27" s="130" t="s">
+      <c r="F27" s="160"/>
+      <c r="G27" s="161" t="s">
         <v>151</v>
       </c>
-      <c r="F27" s="131"/>
-      <c r="G27" s="132" t="s">
-        <v>152</v>
-      </c>
-      <c r="H27" s="133"/>
-      <c r="I27" s="134" t="s">
+      <c r="H27" s="162"/>
+      <c r="I27" s="163" t="s">
         <v>128</v>
       </c>
-      <c r="J27" s="134" t="s">
+      <c r="J27" s="80" t="s">
         <v>136</v>
       </c>
       <c r="K27" s="27"/>
@@ -3070,25 +3257,25 @@
     </row>
     <row r="28" spans="1:21" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="54"/>
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="164" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="111" t="s">
+      <c r="D28" s="128"/>
+      <c r="E28" s="129" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="112"/>
-      <c r="E28" s="123" t="s">
+      <c r="F28" s="130"/>
+      <c r="G28" s="131" t="s">
         <v>155</v>
       </c>
-      <c r="F28" s="124"/>
-      <c r="G28" s="125" t="s">
+      <c r="H28" s="132"/>
+      <c r="I28" s="74" t="s">
         <v>156</v>
       </c>
-      <c r="H28" s="126"/>
-      <c r="I28" s="110" t="s">
-        <v>157</v>
-      </c>
-      <c r="J28" s="110" t="s">
+      <c r="J28" s="82" t="s">
         <v>136</v>
       </c>
       <c r="K28" s="27"/>
@@ -3100,25 +3287,25 @@
     </row>
     <row r="29" spans="1:21" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54"/>
-      <c r="B29" s="122" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="150" t="s">
+      <c r="B29" s="164" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="133" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="134"/>
+      <c r="E29" s="135" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="136"/>
+      <c r="G29" s="137" t="s">
         <v>171</v>
       </c>
-      <c r="D29" s="151"/>
-      <c r="E29" s="152" t="s">
-        <v>172</v>
-      </c>
-      <c r="F29" s="153"/>
-      <c r="G29" s="154" t="s">
-        <v>173</v>
-      </c>
-      <c r="H29" s="155"/>
-      <c r="I29" s="156" t="s">
+      <c r="H29" s="138"/>
+      <c r="I29" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="J29" s="156" t="s">
+      <c r="J29" s="165" t="s">
         <v>136</v>
       </c>
       <c r="K29" s="27"/>
@@ -3130,17 +3317,27 @@
     </row>
     <row r="30" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="54"/>
-      <c r="B30" s="122" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="150"/>
-      <c r="D30" s="151"/>
-      <c r="E30" s="152"/>
-      <c r="F30" s="153"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="155"/>
-      <c r="I30" s="156"/>
-      <c r="J30" s="156"/>
+      <c r="B30" s="164" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="133" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="F30" s="136"/>
+      <c r="G30" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" s="138"/>
+      <c r="I30" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="J30" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
       <c r="R30" s="5"/>
@@ -3150,17 +3347,27 @@
     </row>
     <row r="31" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54"/>
-      <c r="B31" s="122" t="s">
-        <v>160</v>
-      </c>
-      <c r="C31" s="150"/>
-      <c r="D31" s="151"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="155"/>
-      <c r="I31" s="156"/>
-      <c r="J31" s="156"/>
+      <c r="B31" s="164" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="133" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" s="134"/>
+      <c r="E31" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="F31" s="136"/>
+      <c r="G31" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="138"/>
+      <c r="I31" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
       <c r="R31" s="5"/>
@@ -3170,17 +3377,27 @@
     </row>
     <row r="32" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="54"/>
-      <c r="B32" s="122" t="s">
-        <v>161</v>
-      </c>
-      <c r="C32" s="150"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="153"/>
-      <c r="G32" s="154"/>
-      <c r="H32" s="155"/>
-      <c r="I32" s="156"/>
-      <c r="J32" s="156"/>
+      <c r="B32" s="164" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="133" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="134"/>
+      <c r="E32" s="135" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" s="136"/>
+      <c r="G32" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H32" s="138"/>
+      <c r="I32" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K32" s="27"/>
       <c r="L32" s="27"/>
       <c r="R32" s="5"/>
@@ -3190,17 +3407,27 @@
     </row>
     <row r="33" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="54"/>
-      <c r="B33" s="122" t="s">
-        <v>162</v>
-      </c>
-      <c r="C33" s="150"/>
-      <c r="D33" s="151"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="153"/>
-      <c r="G33" s="154"/>
-      <c r="H33" s="155"/>
-      <c r="I33" s="156"/>
-      <c r="J33" s="156"/>
+      <c r="B33" s="164" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="133" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="136"/>
+      <c r="G33" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" s="138"/>
+      <c r="I33" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="J33" s="165" t="s">
+        <v>129</v>
+      </c>
       <c r="K33" s="27"/>
       <c r="L33" s="27"/>
       <c r="R33" s="5"/>
@@ -3210,17 +3437,27 @@
     </row>
     <row r="34" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="54"/>
-      <c r="B34" s="122" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="150"/>
-      <c r="D34" s="151"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="154"/>
-      <c r="H34" s="155"/>
-      <c r="I34" s="156"/>
-      <c r="J34" s="156"/>
+      <c r="B34" s="164" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="133" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="134"/>
+      <c r="E34" s="135" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="136"/>
+      <c r="G34" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H34" s="138"/>
+      <c r="I34" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="J34" s="165" t="s">
+        <v>129</v>
+      </c>
       <c r="K34" s="27"/>
       <c r="L34" s="27"/>
       <c r="R34" s="5"/>
@@ -3230,17 +3467,27 @@
     </row>
     <row r="35" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="54"/>
-      <c r="B35" s="122" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" s="150"/>
-      <c r="D35" s="151"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="153"/>
-      <c r="G35" s="154"/>
-      <c r="H35" s="155"/>
-      <c r="I35" s="156"/>
-      <c r="J35" s="156"/>
+      <c r="B35" s="164" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="133" t="s">
+        <v>182</v>
+      </c>
+      <c r="D35" s="134"/>
+      <c r="E35" s="135" t="s">
+        <v>183</v>
+      </c>
+      <c r="F35" s="136"/>
+      <c r="G35" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H35" s="138"/>
+      <c r="I35" s="86" t="s">
+        <v>130</v>
+      </c>
+      <c r="J35" s="165" t="s">
+        <v>129</v>
+      </c>
       <c r="K35" s="27"/>
       <c r="L35" s="27"/>
       <c r="R35" s="5"/>
@@ -3250,17 +3497,27 @@
     </row>
     <row r="36" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="54"/>
-      <c r="B36" s="122" t="s">
-        <v>165</v>
-      </c>
-      <c r="C36" s="150"/>
-      <c r="D36" s="151"/>
-      <c r="E36" s="152"/>
-      <c r="F36" s="153"/>
-      <c r="G36" s="154"/>
-      <c r="H36" s="155"/>
-      <c r="I36" s="156"/>
-      <c r="J36" s="156"/>
+      <c r="B36" s="164" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="133" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="134"/>
+      <c r="E36" s="135" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="136"/>
+      <c r="G36" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" s="138"/>
+      <c r="I36" s="86" t="s">
+        <v>130</v>
+      </c>
+      <c r="J36" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K36" s="27"/>
       <c r="L36" s="27"/>
       <c r="R36" s="5"/>
@@ -3270,17 +3527,27 @@
     </row>
     <row r="37" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="54"/>
-      <c r="B37" s="122" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="150"/>
-      <c r="D37" s="151"/>
-      <c r="E37" s="152"/>
-      <c r="F37" s="153"/>
-      <c r="G37" s="154"/>
-      <c r="H37" s="155"/>
-      <c r="I37" s="156"/>
-      <c r="J37" s="156"/>
+      <c r="B37" s="164" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="134"/>
+      <c r="E37" s="135" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="136"/>
+      <c r="G37" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="138"/>
+      <c r="I37" s="86" t="s">
+        <v>130</v>
+      </c>
+      <c r="J37" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K37" s="27"/>
       <c r="L37" s="27"/>
       <c r="R37" s="5"/>
@@ -3290,17 +3557,27 @@
     </row>
     <row r="38" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="54"/>
-      <c r="B38" s="122" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="150"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="153"/>
-      <c r="G38" s="154"/>
-      <c r="H38" s="155"/>
-      <c r="I38" s="156"/>
-      <c r="J38" s="156"/>
+      <c r="B38" s="164" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="133" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="134"/>
+      <c r="E38" s="135" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" s="136"/>
+      <c r="G38" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H38" s="138"/>
+      <c r="I38" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="J38" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K38" s="27"/>
       <c r="L38" s="27"/>
       <c r="R38" s="5"/>
@@ -3310,17 +3587,27 @@
     </row>
     <row r="39" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="54"/>
-      <c r="B39" s="122" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="150"/>
-      <c r="D39" s="151"/>
-      <c r="E39" s="152"/>
-      <c r="F39" s="153"/>
-      <c r="G39" s="154"/>
-      <c r="H39" s="155"/>
-      <c r="I39" s="156"/>
-      <c r="J39" s="156"/>
+      <c r="B39" s="164" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="133" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" s="134"/>
+      <c r="E39" s="135" t="s">
+        <v>191</v>
+      </c>
+      <c r="F39" s="136"/>
+      <c r="G39" s="137" t="s">
+        <v>171</v>
+      </c>
+      <c r="H39" s="138"/>
+      <c r="I39" s="86" t="s">
+        <v>130</v>
+      </c>
+      <c r="J39" s="165" t="s">
+        <v>136</v>
+      </c>
       <c r="K39" s="27"/>
       <c r="L39" s="27"/>
       <c r="R39" s="5"/>
@@ -3328,19 +3615,29 @@
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
     </row>
-    <row r="40" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="54"/>
-      <c r="B40" s="122" t="s">
-        <v>169</v>
-      </c>
-      <c r="C40" s="150"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="152"/>
-      <c r="F40" s="153"/>
-      <c r="G40" s="154"/>
-      <c r="H40" s="155"/>
-      <c r="I40" s="156"/>
-      <c r="J40" s="156"/>
+      <c r="B40" s="166" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" s="167" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="168"/>
+      <c r="E40" s="169" t="s">
+        <v>193</v>
+      </c>
+      <c r="F40" s="170"/>
+      <c r="G40" s="171" t="s">
+        <v>171</v>
+      </c>
+      <c r="H40" s="172"/>
+      <c r="I40" s="173" t="s">
+        <v>130</v>
+      </c>
+      <c r="J40" s="174" t="s">
+        <v>136</v>
+      </c>
       <c r="K40" s="27"/>
       <c r="L40" s="27"/>
       <c r="R40" s="5"/>
@@ -3350,17 +3647,15 @@
     </row>
     <row r="41" spans="1:21" s="4" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="54"/>
-      <c r="B41" s="122" t="s">
-        <v>170</v>
-      </c>
-      <c r="C41" s="150"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="152"/>
-      <c r="F41" s="153"/>
-      <c r="G41" s="154"/>
-      <c r="H41" s="155"/>
-      <c r="I41" s="156"/>
-      <c r="J41" s="156"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="149"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="151"/>
+      <c r="F41" s="152"/>
+      <c r="G41" s="153"/>
+      <c r="H41" s="154"/>
+      <c r="I41" s="155"/>
+      <c r="J41" s="155"/>
       <c r="K41" s="27"/>
       <c r="L41" s="27"/>
       <c r="R41" s="5"/>
@@ -3484,7 +3779,7 @@
       <c r="B50" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="121">
+      <c r="C50" s="76">
         <v>43600</v>
       </c>
       <c r="D50" s="24"/>
@@ -3544,17 +3839,12 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G24:H24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="C16:D16"/>
@@ -3563,6 +3853,27 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -3571,22 +3882,6 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -3609,7 +3904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -3717,10 +4012,10 @@
       <c r="A15" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="139" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="96"/>
+      <c r="C15" s="139"/>
       <c r="D15" s="41"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -4064,20 +4359,20 @@
     <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="66"/>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="99"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="142"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="102"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="145"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -4272,30 +4567,30 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
       <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="147" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
+      <c r="D23" s="148"/>
+      <c r="E23" s="148"/>
+      <c r="F23" s="148"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="104"/>
+      <c r="B24" s="147"/>
       <c r="C24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="12"/>

</xml_diff>